<commit_message>
test_tc004 excel see bug fixed & some improvements
</commit_message>
<xml_diff>
--- a/assets/test.xlsx
+++ b/assets/test.xlsx
@@ -431,7 +431,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="11" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Not Seen</t>
+          <t>Seen</t>
         </is>
       </c>
     </row>

</xml_diff>